<commit_message>
Fixed obj function bug
</commit_message>
<xml_diff>
--- a/Code/Optimiser/Multi SolCheck.xlsx
+++ b/Code/Optimiser/Multi SolCheck.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Optimiser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7F1F03D-79C4-4C59-BE9D-76759B13BCC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878DD571-ABD7-4AC8-A484-4D27172A6DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1216E67F-FE2E-4197-BF88-EB74DB65ED3B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Availability</t>
   </si>
@@ -104,16 +104,7 @@
     <t>Breakage cost</t>
   </si>
   <si>
-    <t>Broken at end</t>
-  </si>
-  <si>
-    <t>Rep value</t>
-  </si>
-  <si>
-    <t>Failure values</t>
-  </si>
-  <si>
-    <t>FIND OUT DIFFERENCES</t>
+    <t>Fails at end</t>
   </si>
 </sst>
 </file>
@@ -474,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FA0CDE-058B-4AE7-A06C-36CDD84BAEFC}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,13 +478,13 @@
     <col min="7" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,7 +515,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -541,10 +532,10 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -552,7 +543,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -561,7 +552,7 @@
         <v>388800</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -569,7 +560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -577,29 +568,22 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <f>I25+J25+L25</f>
-        <v>19142400</v>
-      </c>
-      <c r="C10">
-        <f>N26+E25*B5*B7+C25*E2+D25*E3-SUMPRODUCT(F13:F24,O13:O24)</f>
-        <v>17198400</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>18596000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -636,14 +620,8 @@
       <c r="L12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -686,16 +664,8 @@
         <f>K13*$B$6</f>
         <v>0</v>
       </c>
-      <c r="N13">
-        <f>B13*(11-A13)</f>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f>$B$6*(11-A13)</f>
-        <v>4276800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -738,16 +708,8 @@
         <f t="shared" ref="L14:L24" si="4">K14*$B$6</f>
         <v>388800</v>
       </c>
-      <c r="N14">
-        <f t="shared" ref="N14:N24" si="5">B14*(11-A14)</f>
-        <v>10</v>
-      </c>
-      <c r="O14">
-        <f t="shared" ref="O14:O24" si="6">$B$6*(11-A14)</f>
-        <v>3888000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -783,23 +745,15 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K24" si="7">K14+B15-F15</f>
+        <f t="shared" ref="K15:K24" si="5">K14+B15-F15</f>
         <v>5</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
         <v>1944000</v>
       </c>
-      <c r="N15">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="6"/>
-        <v>3499200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -835,23 +789,15 @@
         <v>213840</v>
       </c>
       <c r="K16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
         <v>777600</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="6"/>
-        <v>3110400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -887,23 +833,15 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L17">
         <f t="shared" si="4"/>
         <v>388800</v>
       </c>
-      <c r="N17">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="6"/>
-        <v>2721600</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -939,23 +877,15 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L18">
         <f t="shared" si="4"/>
         <v>2721600</v>
       </c>
-      <c r="N18">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="6"/>
-        <v>2332800</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -991,23 +921,15 @@
         <v>194400</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L19">
         <f t="shared" si="4"/>
         <v>3110400</v>
       </c>
-      <c r="N19">
-        <f t="shared" si="5"/>
-        <v>40</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="6"/>
-        <v>1944000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1043,23 +965,15 @@
         <v>187920</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L20">
         <f t="shared" si="4"/>
         <v>777600</v>
       </c>
-      <c r="N20">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="6"/>
-        <v>1555200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1095,23 +1009,15 @@
         <v>51840</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="6"/>
-        <v>1166400</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1147,23 +1053,15 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L22">
         <f t="shared" si="4"/>
         <v>1555200</v>
       </c>
-      <c r="N22">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="6"/>
-        <v>777600</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1199,23 +1097,15 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L23">
         <f t="shared" si="4"/>
         <v>1166400</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="6"/>
-        <v>388800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -1223,51 +1113,43 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>696</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>432</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>620000</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
-        <v>1944000</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1276,50 +1158,40 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:I25" si="8">SUM(C13:C24)</f>
-        <v>6</v>
+        <f t="shared" ref="C25:I25" si="6">SUM(C13:C24)</f>
+        <v>7</v>
       </c>
       <c r="D25">
-        <f t="shared" si="8"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="E25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="F25">
-        <f t="shared" si="8"/>
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>31</v>
       </c>
       <c r="G25">
-        <f t="shared" si="8"/>
-        <v>3696</v>
+        <f t="shared" si="6"/>
+        <v>4392</v>
       </c>
       <c r="H25">
-        <f t="shared" si="8"/>
-        <v>1232</v>
+        <f t="shared" si="6"/>
+        <v>1664</v>
       </c>
       <c r="I25">
-        <f t="shared" si="8"/>
-        <v>3720000</v>
+        <f t="shared" si="6"/>
+        <v>4340000</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25" si="9">SUM(J13:J24)</f>
+        <f t="shared" ref="J25" si="7">SUM(J13:J24)</f>
         <v>648000</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25" si="10">SUM(L13:L24)</f>
-        <v>14774400</v>
-      </c>
-      <c r="N25">
-        <f t="shared" ref="N25" si="11">SUM(N13:N24)</f>
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N26">
-        <f>164*B6</f>
-        <v>63763200</v>
+        <f t="shared" ref="L25" si="8">SUM(L13:L24)</f>
+        <v>13608000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
INCOMPLETE Added new level to model
</commit_message>
<xml_diff>
--- a/Code/Optimiser/Multi SolCheck.xlsx
+++ b/Code/Optimiser/Multi SolCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Optimiser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878DD571-ABD7-4AC8-A484-4D27172A6DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F5DC48-B1A9-4441-84CC-9827E1BD07CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1216E67F-FE2E-4197-BF88-EB74DB65ED3B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="30">
   <si>
     <t>Availability</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>Fails at end</t>
+  </si>
+  <si>
+    <t>Scenario 0</t>
+  </si>
+  <si>
+    <t>Scenario 4</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Total Obj</t>
   </si>
 </sst>
 </file>
@@ -465,14 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FA0CDE-058B-4AE7-A06C-36CDD84BAEFC}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:F24"/>
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -573,104 +592,78 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B10">
-        <f>I25+J25+L25</f>
-        <v>18596000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+        <f>AVERAGE(C12,C28,C44,C60,C76)</f>
+        <v>15355520</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <f>I26+J26+L26</f>
+        <v>11097600</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f>C13*$B$2 - E13*$C$2-F13*$D$2</f>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f>C13*$B$3 - E13*$C$3-F13*$D$3</f>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f>C13*$E$2+D13*$E$3</f>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f>E13*$B$7*$B$5</f>
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f>B13-F13</f>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f>K13*$B$6</f>
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -685,36 +678,36 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:G24" si="0">C14*$B$2 - E14*$C$2-F14*$D$2</f>
+        <f>C14*$B$2 - E14*$C$2-F14*$D$2</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14:H24" si="1">C14*$B$3 - E14*$C$3-F14*$D$3</f>
+        <f>D14*$B$3 - E14*$C$3-F14*$D$3</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I24" si="2">C14*$E$2+D14*$E$3</f>
+        <f>C14*$E$2+D14*$E$3</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" ref="J14:J24" si="3">E14*$B$7*$B$5</f>
+        <f>E14*$B$7*$B$5</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>K13+B14-F14</f>
-        <v>1</v>
+        <f>B14-F14</f>
+        <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:L24" si="4">K14*$B$6</f>
-        <v>388800</v>
+        <f>K14*$B$6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -729,36 +722,36 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G15:G25" si="0">C15*$B$2 - E15*$C$2-F15*$D$2</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H15:H25" si="1">D15*$B$3 - E15*$C$3-F15*$D$3</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="I15:I25" si="2">C15*$E$2+D15*$E$3</f>
         <v>0</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J15:J25" si="3">E15*$B$7*$B$5</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K24" si="5">K14+B15-F15</f>
-        <v>5</v>
+        <f>K14+B15-F15</f>
+        <v>2</v>
       </c>
       <c r="L15">
-        <f t="shared" si="4"/>
-        <v>1944000</v>
+        <f t="shared" ref="L15:L25" si="4">K15*$B$6</f>
+        <v>777600</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -767,18 +760,18 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>548</v>
+        <v>704</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>448</v>
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
@@ -786,47 +779,47 @@
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>213840</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" ref="K16:K25" si="5">K15+B16-F16</f>
+        <v>0</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>777600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>704</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>448</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>620000</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
@@ -834,19 +827,19 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <f t="shared" si="4"/>
-        <v>388800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -878,19 +871,19 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L18">
         <f t="shared" si="4"/>
-        <v>2721600</v>
+        <v>1166400</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -899,18 +892,18 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>544</v>
+        <v>696</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>432</v>
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
@@ -918,67 +911,67 @@
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>194400</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L19">
         <f t="shared" si="4"/>
-        <v>3110400</v>
+        <v>777600</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
-        <v>540</v>
+        <f>C20*$B$2 - E20*$C$2-F20*$D$2</f>
+        <v>440</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>620000</v>
+        <v>740000</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>187920</v>
+        <v>427680</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L20">
         <f t="shared" si="4"/>
-        <v>777600</v>
+        <v>1555200</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -987,18 +980,18 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>672</v>
+        <v>552</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>352</v>
+        <v>8</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
@@ -1006,47 +999,47 @@
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>51840</v>
+        <v>220320</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1555200</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>4</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>688</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>416</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>620000</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
@@ -1054,43 +1047,43 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <f t="shared" si="4"/>
-        <v>1555200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>688</v>
+        <v>0</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>416</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>620000</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
@@ -1098,19 +1091,19 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <f t="shared" si="4"/>
-        <v>1166400</v>
+        <v>777600</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1122,15 +1115,15 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>432</v>
+        <v>448</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
@@ -1142,56 +1135,2592 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
-        <v>777600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
-        <f>SUM(B13:B24)</f>
-        <v>33</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ref="C25:I25" si="6">SUM(C13:C24)</f>
-        <v>7</v>
-      </c>
-      <c r="D25">
+      <c r="B26">
+        <f>SUM(B14:B25)</f>
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:I26" si="6">SUM(C14:C25)</f>
+        <v>6</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="G25">
+        <v>17</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="6"/>
-        <v>4392</v>
-      </c>
-      <c r="H25">
+        <v>3784</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="6"/>
-        <v>1664</v>
-      </c>
-      <c r="I25">
+        <v>1888</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="6"/>
-        <v>4340000</v>
-      </c>
-      <c r="J25">
-        <f t="shared" ref="J25" si="7">SUM(J13:J24)</f>
+        <v>3840000</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26" si="7">SUM(J14:J25)</f>
         <v>648000</v>
       </c>
-      <c r="L25">
-        <f t="shared" ref="L25" si="8">SUM(L13:L24)</f>
-        <v>13608000</v>
+      <c r="L26">
+        <f t="shared" ref="L26" si="8">SUM(L14:L25)</f>
+        <v>6609600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <f>I42+J42+L42</f>
+        <v>14050400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>C30*$B$2 - E30*$C$2-F30*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f>D30*$B$3 - E30*$C$3-F30*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>C30*$E$2+D30*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f>E30*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>B30-F30</f>
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <f>K30*$B$6</f>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G41" si="9">C31*$B$2 - E31*$C$2-F31*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H41" si="10">D31*$B$3 - E31*$C$3-F31*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:I41" si="11">C31*$E$2+D31*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ref="J31:J41" si="12">E31*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f>K30+B31-F31</f>
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ref="L31:L41" si="13">K31*$B$6</f>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="9"/>
+        <v>696</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="10"/>
+        <v>432</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:K41" si="14">K31+B32-F32</f>
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="13"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>688</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>416</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="13"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>66</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>448</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="11"/>
+        <v>740000</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="12"/>
+        <v>427680</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="13"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>34</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>552</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="12"/>
+        <v>220320</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="13"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>704</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="10"/>
+        <v>448</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="13"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>704</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="10"/>
+        <v>448</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="13"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="9"/>
+        <v>696</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="10"/>
+        <v>432</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="11"/>
+        <v>620000</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="13"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <f>SUM(B30:B41)</f>
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:J42" si="15">SUM(C30:C41)</f>
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="15"/>
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="15"/>
+        <v>4488</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="15"/>
+        <v>2336</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="15"/>
+        <v>4460000</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="15"/>
+        <v>648000</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42" si="16">SUM(L30:L41)</f>
+        <v>8942400</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <f>I58+J58+L58</f>
+        <v>17623200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f>C46*$B$2 - E46*$C$2-F46*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <f>D46*$B$3 - E46*$C$3-F46*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f>C46*$E$2+D46*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f>E46*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <f>B46-F46</f>
+        <v>2</v>
+      </c>
+      <c r="L46">
+        <f>K46*$B$6</f>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47:G57" si="17">C47*$B$2 - E47*$C$2-F47*$D$2</f>
+        <v>704</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ref="H47:H57" si="18">D47*$B$3 - E47*$C$3-F47*$D$3</f>
+        <v>448</v>
+      </c>
+      <c r="I47">
+        <f t="shared" ref="I47:I57" si="19">C47*$E$2+D47*$E$3</f>
+        <v>620000</v>
+      </c>
+      <c r="J47">
+        <f t="shared" ref="J47:J57" si="20">E47*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f>K46+B47-F47</f>
+        <v>3</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ref="L47:L57" si="21">K47*$B$6</f>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="17"/>
+        <v>696</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="18"/>
+        <v>432</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ref="K48:K57" si="22">K47+B48-F48</f>
+        <v>2</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="21"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="17"/>
+        <v>704</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="18"/>
+        <v>448</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="21"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="21"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="17"/>
+        <v>688</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="18"/>
+        <v>416</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="21"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>66</v>
+      </c>
+      <c r="F52">
+        <v>3</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="17"/>
+        <v>432</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="18"/>
+        <v>120</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="19"/>
+        <v>740000</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="20"/>
+        <v>427680</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="21"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>34</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="17"/>
+        <v>552</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="20"/>
+        <v>220320</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="21"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>8</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="17"/>
+        <v>696</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="18"/>
+        <v>432</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="21"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="17"/>
+        <v>696</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="18"/>
+        <v>432</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="21"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="17"/>
+        <v>704</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="18"/>
+        <v>448</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="19"/>
+        <v>620000</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="21"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="21"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58">
+        <f>SUM(B46:B57)</f>
+        <v>27</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:J58" si="23">SUM(C46:C57)</f>
+        <v>9</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="23"/>
+        <v>100</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="23"/>
+        <v>26</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="23"/>
+        <v>5872</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="23"/>
+        <v>3184</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="23"/>
+        <v>5700000</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="23"/>
+        <v>648000</v>
+      </c>
+      <c r="L58">
+        <f t="shared" ref="L58" si="24">SUM(L46:L57)</f>
+        <v>11275200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <f>I74+J74+L74</f>
+        <v>17392000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <f>C62*$B$2 - E62*$C$2-F62*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <f>D62*$B$3 - E62*$C$3-F62*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <f>C62*$E$2+D62*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <f>E62*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <f>B62-F62</f>
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <f>K62*$B$6</f>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ref="G63:G73" si="25">C63*$B$2 - E63*$C$2-F63*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <f t="shared" ref="H63:H73" si="26">D63*$B$3 - E63*$C$3-F63*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f t="shared" ref="I63:I73" si="27">C63*$E$2+D63*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <f t="shared" ref="J63:J73" si="28">E63*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <f>K62+B63-F63</f>
+        <v>3</v>
+      </c>
+      <c r="L63">
+        <f t="shared" ref="L63:L73" si="29">K63*$B$6</f>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>3</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="25"/>
+        <v>696</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="26"/>
+        <v>432</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <f t="shared" ref="K64:K73" si="30">K63+B64-F64</f>
+        <v>4</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="29"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>4</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="25"/>
+        <v>688</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="26"/>
+        <v>416</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="29"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="25"/>
+        <v>704</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="26"/>
+        <v>448</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="29"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>3</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="25"/>
+        <v>696</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="26"/>
+        <v>432</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="29"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>66</v>
+      </c>
+      <c r="F68">
+        <v>3</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="25"/>
+        <v>432</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="26"/>
+        <v>120</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="27"/>
+        <v>740000</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="28"/>
+        <v>427680</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="29"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>7</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>34</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="25"/>
+        <v>568</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="26"/>
+        <v>40</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="28"/>
+        <v>220320</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>8</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="29"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>9</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="25"/>
+        <v>704</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="26"/>
+        <v>448</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="30"/>
+        <v>4</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="29"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="25"/>
+        <v>688</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="26"/>
+        <v>416</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="27"/>
+        <v>620000</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="29"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>11</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="30"/>
+        <v>5</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="29"/>
+        <v>1944000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74">
+        <f>SUM(B62:B73)</f>
+        <v>28</v>
+      </c>
+      <c r="C74">
+        <f t="shared" ref="C74:J74" si="31">SUM(C62:C73)</f>
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="31"/>
+        <v>100</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="31"/>
+        <v>23</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="31"/>
+        <v>5176</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="31"/>
+        <v>2752</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="31"/>
+        <v>5080000</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="31"/>
+        <v>648000</v>
+      </c>
+      <c r="L74">
+        <f t="shared" ref="L74" si="32">SUM(L62:L73)</f>
+        <v>11664000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <f>I90+J90+L90</f>
+        <v>16614400</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <f>C78*$B$2 - E78*$C$2-F78*$D$2</f>
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <f>D78*$B$3 - E78*$C$3-F78*$D$3</f>
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <f>C78*$E$2+D78*$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <f>E78*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <f>B78-F78</f>
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <f>K78*$B$6</f>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>2</v>
+      </c>
+      <c r="G79">
+        <f t="shared" ref="G79:G89" si="33">C79*$B$2 - E79*$C$2-F79*$D$2</f>
+        <v>704</v>
+      </c>
+      <c r="H79">
+        <f t="shared" ref="H79:H89" si="34">D79*$B$3 - E79*$C$3-F79*$D$3</f>
+        <v>448</v>
+      </c>
+      <c r="I79">
+        <f t="shared" ref="I79:I89" si="35">C79*$E$2+D79*$E$3</f>
+        <v>620000</v>
+      </c>
+      <c r="J79">
+        <f t="shared" ref="J79:J89" si="36">E79*$B$7*$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <f>K78+B79-F79</f>
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <f t="shared" ref="L79:L89" si="37">K79*$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <f t="shared" ref="K80:K89" si="38">K79+B80-F80</f>
+        <v>4</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="37"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>4</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="33"/>
+        <v>688</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="34"/>
+        <v>416</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="38"/>
+        <v>5</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="37"/>
+        <v>1944000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="33"/>
+        <v>680</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="34"/>
+        <v>400</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="37"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="37"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>66</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="33"/>
+        <v>432</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="34"/>
+        <v>120</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="35"/>
+        <v>740000</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="36"/>
+        <v>427680</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="37"/>
+        <v>388800</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>34</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="33"/>
+        <v>576</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="34"/>
+        <v>56</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="36"/>
+        <v>220320</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="38"/>
+        <v>2</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="37"/>
+        <v>777600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>8</v>
+      </c>
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>2</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="33"/>
+        <v>704</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="34"/>
+        <v>448</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="38"/>
+        <v>4</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="37"/>
+        <v>1555200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>4</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="33"/>
+        <v>688</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="34"/>
+        <v>416</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="37"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>11</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="33"/>
+        <v>696</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="34"/>
+        <v>432</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="35"/>
+        <v>620000</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="37"/>
+        <v>1166400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90">
+        <f>SUM(B78:B89)</f>
+        <v>27</v>
+      </c>
+      <c r="C90">
+        <f t="shared" ref="C90:J90" si="39">SUM(C78:C89)</f>
+        <v>8</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="39"/>
+        <v>9</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="39"/>
+        <v>100</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="39"/>
+        <v>24</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="39"/>
+        <v>5168</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="39"/>
+        <v>2736</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="39"/>
+        <v>5080000</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="39"/>
+        <v>648000</v>
+      </c>
+      <c r="L90">
+        <f t="shared" ref="L90" si="40">SUM(L78:L89)</f>
+        <v>10886400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>